<commit_message>
update data; add spatial data
</commit_message>
<xml_diff>
--- a/data/APO - Water quality.xlsx
+++ b/data/APO - Water quality.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD/Projekte/apo-sub-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C64E97E-8F3B-2343-9724-349CEE1C125C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{974CE16C-828E-374F-858E-53C1F705814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="33600" activeTab="1" xr2:uid="{C5E9C466-93C4-574F-B63C-9AC7A4C519C5}"/>
+    <workbookView xWindow="1260" yWindow="500" windowWidth="19740" windowHeight="33100" activeTab="1" xr2:uid="{C5E9C466-93C4-574F-B63C-9AC7A4C519C5}"/>
   </bookViews>
   <sheets>
     <sheet name="important Notes" sheetId="3" r:id="rId1"/>
@@ -1485,7 +1485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="397">
   <si>
     <t>Macronutrients</t>
   </si>
@@ -2427,6 +2427,255 @@
   </si>
   <si>
     <t>MAK</t>
+  </si>
+  <si>
+    <t>Stadtwerke Düsseldorf</t>
+  </si>
+  <si>
+    <t>Düsseldorf</t>
+  </si>
+  <si>
+    <t>swa Trinkwaasser</t>
+  </si>
+  <si>
+    <t>Augsburg</t>
+  </si>
+  <si>
+    <t>48.37691953678279, 10.885124703686214</t>
+  </si>
+  <si>
+    <t>51.227462177725485, 6.774522887786429</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Wasserversorgung Liechtensteiner Unterland</t>
+  </si>
+  <si>
+    <t>Gamprin-Bendern</t>
+  </si>
+  <si>
+    <t>47.21220599170113, 9.508231723996175</t>
+  </si>
+  <si>
+    <t>WN05, 45 Mauren, Lachenstrasse 40</t>
+  </si>
+  <si>
+    <t>SWE</t>
+  </si>
+  <si>
+    <t>Mischwasser</t>
+  </si>
+  <si>
+    <t>Erfurt</t>
+  </si>
+  <si>
+    <t>50.96163874501972, 11.00019847649089</t>
+  </si>
+  <si>
+    <t>avacon</t>
+  </si>
+  <si>
+    <t>Lüneburg</t>
+  </si>
+  <si>
+    <t>53.24780050481698, 10.392485041796528</t>
+  </si>
+  <si>
+    <t>FWA</t>
+  </si>
+  <si>
+    <t>Frankfurt an der Oder</t>
+  </si>
+  <si>
+    <t>52.34824800786877, 14.45787844599074</t>
+  </si>
+  <si>
+    <t>Lausitzer Wasser</t>
+  </si>
+  <si>
+    <t>Fehrower Weg</t>
+  </si>
+  <si>
+    <t>Cottbus</t>
+  </si>
+  <si>
+    <t>51.78306291392819, 14.332748740843407</t>
+  </si>
+  <si>
+    <t>Zweckverband Wasserversorgung &amp; Abwasserbeseitigung Usedom</t>
+  </si>
+  <si>
+    <t>Wasserwerk Usedom</t>
+  </si>
+  <si>
+    <t>Usedom</t>
+  </si>
+  <si>
+    <t>53.93314229156935, 14.089066847581185</t>
+  </si>
+  <si>
+    <t>Hümmling Wasserverband</t>
+  </si>
+  <si>
+    <t>Wasserwerk Surwold</t>
+  </si>
+  <si>
+    <t>Surwold</t>
+  </si>
+  <si>
+    <t>53.00566461904555, 7.494061736114276</t>
+  </si>
+  <si>
+    <t>HB Berndorf</t>
+  </si>
+  <si>
+    <t>Verbandsgemeinde Gerolstein</t>
+  </si>
+  <si>
+    <t>Gerolstein</t>
+  </si>
+  <si>
+    <t>50.22081953012955, 6.633580506707629</t>
+  </si>
+  <si>
+    <t>STAWAG</t>
+  </si>
+  <si>
+    <t>Härtebereich 1</t>
+  </si>
+  <si>
+    <t>Aachen</t>
+  </si>
+  <si>
+    <t>50.799770983519316, 6.090636595164506</t>
+  </si>
+  <si>
+    <t>Stadtwerke Baden-Baden</t>
+  </si>
+  <si>
+    <t>Baden-Baden</t>
+  </si>
+  <si>
+    <t>48.789514973338584, 8.24093411253014</t>
+  </si>
+  <si>
+    <t>Grundwasser</t>
+  </si>
+  <si>
+    <t>Quellwasser</t>
+  </si>
+  <si>
+    <t>Kemptener Kommunalunternehmen</t>
+  </si>
+  <si>
+    <t>Mittel- und Niederzone</t>
+  </si>
+  <si>
+    <t>Kempten</t>
+  </si>
+  <si>
+    <t>47.72508426221937, 10.308332388766141</t>
+  </si>
+  <si>
+    <t>Salzburg AG</t>
+  </si>
+  <si>
+    <t>Behälter Mönchsberg</t>
+  </si>
+  <si>
+    <t>Salzburg</t>
+  </si>
+  <si>
+    <t>47.836883470180986, 13.062113178347834</t>
+  </si>
+  <si>
+    <t>Stadtwerke Klagenfurt AG</t>
+  </si>
+  <si>
+    <t>Pumpanlage Zwirnawald</t>
+  </si>
+  <si>
+    <t>Klagenfurt</t>
+  </si>
+  <si>
+    <t>46.6786095104281, 14.3292087136818</t>
+  </si>
+  <si>
+    <t>Stadtwerke Kufstein</t>
+  </si>
+  <si>
+    <t>Tiefbrunnen Fürhölzl</t>
+  </si>
+  <si>
+    <t>Kufstein</t>
+  </si>
+  <si>
+    <t>47.56132432685829, 12.131185933964833</t>
+  </si>
+  <si>
+    <t>Linz AG</t>
+  </si>
+  <si>
+    <t>Hafen</t>
+  </si>
+  <si>
+    <t>Linz</t>
+  </si>
+  <si>
+    <t>48.329222431517636, 14.286110320787243</t>
+  </si>
+  <si>
+    <t>Graz Holding</t>
+  </si>
+  <si>
+    <t>Brunnen</t>
+  </si>
+  <si>
+    <t>Eisenerz</t>
+  </si>
+  <si>
+    <t>47.54387168914886, 14.893798974015267</t>
+  </si>
+  <si>
+    <t>WVV</t>
+  </si>
+  <si>
+    <t>Hochbehälter Zellingen</t>
+  </si>
+  <si>
+    <t>Würzburg</t>
+  </si>
+  <si>
+    <t>49.817346113608544, 9.959340566631953</t>
+  </si>
+  <si>
+    <t>Stockholm Vatten och avfall</t>
+  </si>
+  <si>
+    <t>Stockholm</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>59.46998959413194, 18.08157822419211</t>
+  </si>
+  <si>
+    <t>Norsborg</t>
+  </si>
+  <si>
+    <t>Lovö</t>
+  </si>
+  <si>
+    <t>57.70853071593066, 11.972176149878901</t>
+  </si>
+  <si>
+    <t>Göteborg</t>
+  </si>
+  <si>
+    <t>Göteborgs Stad</t>
   </si>
 </sst>
 </file>
@@ -2808,8 +3057,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97C8753E-B248-414E-8E09-FCA8EAD9E6A1}" name="Tabelle1" displayName="Tabelle1" ref="A2:AU99" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A2:AU99" xr:uid="{97C8753E-B248-414E-8E09-FCA8EAD9E6A1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97C8753E-B248-414E-8E09-FCA8EAD9E6A1}" name="Tabelle1" displayName="Tabelle1" ref="A2:AU122" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A2:AU122" xr:uid="{97C8753E-B248-414E-8E09-FCA8EAD9E6A1}"/>
   <tableColumns count="47">
     <tableColumn id="1" xr3:uid="{C558097B-EFFD-1E4D-9DAB-5449764A12C3}" name="Reference_ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{2354C398-FE28-B547-9546-B8AAC399AADA}" name="Location" dataDxfId="5"/>
@@ -3191,13 +3440,13 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:BB99"/>
+  <dimension ref="A1:BB122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A100" sqref="A100"/>
+      <selection pane="bottomRight" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13698,6 +13947,2446 @@
         <v>93</v>
       </c>
     </row>
+    <row r="100" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H100">
+        <v>7.6</v>
+      </c>
+      <c r="I100">
+        <v>723</v>
+      </c>
+      <c r="J100">
+        <v>0.02</v>
+      </c>
+      <c r="K100" t="s">
+        <v>92</v>
+      </c>
+      <c r="L100">
+        <v>0.02</v>
+      </c>
+      <c r="M100" t="s">
+        <v>92</v>
+      </c>
+      <c r="N100">
+        <v>10.9</v>
+      </c>
+      <c r="O100" t="s">
+        <v>93</v>
+      </c>
+      <c r="P100">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>92</v>
+      </c>
+      <c r="R100">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="S100" t="s">
+        <v>93</v>
+      </c>
+      <c r="T100">
+        <v>84</v>
+      </c>
+      <c r="U100" t="s">
+        <v>93</v>
+      </c>
+      <c r="V100">
+        <v>12</v>
+      </c>
+      <c r="W100" t="s">
+        <v>93</v>
+      </c>
+      <c r="X100">
+        <v>57</v>
+      </c>
+      <c r="Y100" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z100">
+        <v>0.02</v>
+      </c>
+      <c r="AA100" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD100">
+        <v>0.03</v>
+      </c>
+      <c r="AE100" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF100">
+        <v>0.02</v>
+      </c>
+      <c r="AG100" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH100">
+        <v>0.06</v>
+      </c>
+      <c r="AI100" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL100">
+        <v>2E-3</v>
+      </c>
+      <c r="AM100" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN100">
+        <v>44</v>
+      </c>
+      <c r="AO100" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP100">
+        <v>80</v>
+      </c>
+      <c r="AQ100" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR100">
+        <v>0.02</v>
+      </c>
+      <c r="AS100" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="101" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="H101">
+        <v>7.7</v>
+      </c>
+      <c r="I101">
+        <v>441</v>
+      </c>
+      <c r="J101">
+        <v>0.05</v>
+      </c>
+      <c r="K101" t="s">
+        <v>92</v>
+      </c>
+      <c r="L101">
+        <v>0.05</v>
+      </c>
+      <c r="M101" t="s">
+        <v>92</v>
+      </c>
+      <c r="N101">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="O101" t="s">
+        <v>93</v>
+      </c>
+      <c r="R101">
+        <v>1</v>
+      </c>
+      <c r="S101" t="s">
+        <v>93</v>
+      </c>
+      <c r="T101">
+        <f>AVERAGE(63,65)</f>
+        <v>64</v>
+      </c>
+      <c r="U101" t="s">
+        <v>93</v>
+      </c>
+      <c r="V101">
+        <f>AVERAGE(18,19)</f>
+        <v>18.5</v>
+      </c>
+      <c r="W101" t="s">
+        <v>93</v>
+      </c>
+      <c r="X101">
+        <v>23.1</v>
+      </c>
+      <c r="Y101" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z101">
+        <v>0.02</v>
+      </c>
+      <c r="AA101" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD101">
+        <v>0.2</v>
+      </c>
+      <c r="AE101" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF101">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG101" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH101">
+        <v>0.1</v>
+      </c>
+      <c r="AI101" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL101">
+        <v>2E-3</v>
+      </c>
+      <c r="AM101" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN101">
+        <v>5</v>
+      </c>
+      <c r="AO101" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP101">
+        <v>6.2</v>
+      </c>
+      <c r="AQ101" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR101">
+        <v>0.02</v>
+      </c>
+      <c r="AS101" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT101">
+        <v>0.5</v>
+      </c>
+      <c r="AU101" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="H102">
+        <v>7.9</v>
+      </c>
+      <c r="I102">
+        <v>527</v>
+      </c>
+      <c r="J102">
+        <v>0.01</v>
+      </c>
+      <c r="K102" t="s">
+        <v>92</v>
+      </c>
+      <c r="L102">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M102" t="s">
+        <v>92</v>
+      </c>
+      <c r="N102">
+        <v>2.5</v>
+      </c>
+      <c r="O102" t="s">
+        <v>93</v>
+      </c>
+      <c r="P102">
+        <v>0.01</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>92</v>
+      </c>
+      <c r="R102">
+        <v>2.7</v>
+      </c>
+      <c r="S102" t="s">
+        <v>93</v>
+      </c>
+      <c r="T102">
+        <v>71.7</v>
+      </c>
+      <c r="U102" t="s">
+        <v>93</v>
+      </c>
+      <c r="V102">
+        <v>43.3</v>
+      </c>
+      <c r="W102" t="s">
+        <v>93</v>
+      </c>
+      <c r="X102">
+        <v>97.5</v>
+      </c>
+      <c r="Y102" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP102">
+        <v>1.4</v>
+      </c>
+      <c r="AQ102" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT102">
+        <v>0.24</v>
+      </c>
+      <c r="AU102" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="103" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D103" s="5">
+        <v>2022</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="H103">
+        <v>7.9</v>
+      </c>
+      <c r="I103">
+        <v>489</v>
+      </c>
+      <c r="N103">
+        <v>11.2</v>
+      </c>
+      <c r="O103" t="s">
+        <v>93</v>
+      </c>
+      <c r="R103">
+        <v>3.4</v>
+      </c>
+      <c r="S103" t="s">
+        <v>93</v>
+      </c>
+      <c r="T103">
+        <v>66</v>
+      </c>
+      <c r="U103" t="s">
+        <v>93</v>
+      </c>
+      <c r="V103">
+        <v>11.9</v>
+      </c>
+      <c r="W103" t="s">
+        <v>93</v>
+      </c>
+      <c r="X103">
+        <v>85.6</v>
+      </c>
+      <c r="Y103" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z103">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AA103" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF103">
+        <v>1E-3</v>
+      </c>
+      <c r="AG103" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN103">
+        <v>14.9</v>
+      </c>
+      <c r="AO103" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP103">
+        <v>22</v>
+      </c>
+      <c r="AQ103" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR103">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AS103" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="D104" s="5">
+        <v>2022</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="H104">
+        <v>8.01</v>
+      </c>
+      <c r="I104">
+        <v>242</v>
+      </c>
+      <c r="J104">
+        <v>0.04</v>
+      </c>
+      <c r="K104" t="s">
+        <v>92</v>
+      </c>
+      <c r="L104">
+        <v>0.01</v>
+      </c>
+      <c r="M104" t="s">
+        <v>92</v>
+      </c>
+      <c r="N104">
+        <v>0.3</v>
+      </c>
+      <c r="O104" t="s">
+        <v>92</v>
+      </c>
+      <c r="R104">
+        <v>1.6</v>
+      </c>
+      <c r="S104" t="s">
+        <v>93</v>
+      </c>
+      <c r="T104">
+        <v>33.9</v>
+      </c>
+      <c r="U104" t="s">
+        <v>93</v>
+      </c>
+      <c r="V104">
+        <v>11.5</v>
+      </c>
+      <c r="W104" t="s">
+        <v>93</v>
+      </c>
+      <c r="X104">
+        <v>8</v>
+      </c>
+      <c r="Y104" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z104">
+        <v>2.3E-2</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF104">
+        <v>1E-3</v>
+      </c>
+      <c r="AG104" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN104">
+        <v>11.5</v>
+      </c>
+      <c r="AO104" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP104">
+        <v>18.5</v>
+      </c>
+      <c r="AQ104" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="105" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="D105" s="5">
+        <v>2022</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="H105">
+        <v>7.49</v>
+      </c>
+      <c r="I105">
+        <v>813</v>
+      </c>
+      <c r="J105">
+        <v>0.05</v>
+      </c>
+      <c r="K105" t="s">
+        <v>92</v>
+      </c>
+      <c r="N105">
+        <v>0.9</v>
+      </c>
+      <c r="O105" t="s">
+        <v>93</v>
+      </c>
+      <c r="R105">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="S105" t="s">
+        <v>93</v>
+      </c>
+      <c r="T105">
+        <v>110</v>
+      </c>
+      <c r="U105" t="s">
+        <v>93</v>
+      </c>
+      <c r="V105">
+        <v>14.16</v>
+      </c>
+      <c r="W105" t="s">
+        <v>93</v>
+      </c>
+      <c r="X105">
+        <v>202</v>
+      </c>
+      <c r="Y105" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z105">
+        <v>0.02</v>
+      </c>
+      <c r="AA105" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF105">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG105" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH105">
+        <v>0.05</v>
+      </c>
+      <c r="AI105" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN105">
+        <v>29.2</v>
+      </c>
+      <c r="AO105" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP105">
+        <v>39.6</v>
+      </c>
+      <c r="AQ105" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR105">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AS105" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT105">
+        <v>4.63</v>
+      </c>
+      <c r="AU105" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="106" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="D106" s="5">
+        <v>2022</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="H106">
+        <v>7.64</v>
+      </c>
+      <c r="I106">
+        <v>599</v>
+      </c>
+      <c r="J106">
+        <v>0.1</v>
+      </c>
+      <c r="K106" t="s">
+        <v>92</v>
+      </c>
+      <c r="L106">
+        <v>0.01</v>
+      </c>
+      <c r="M106" t="s">
+        <v>92</v>
+      </c>
+      <c r="N106">
+        <v>2.4</v>
+      </c>
+      <c r="O106" t="s">
+        <v>93</v>
+      </c>
+      <c r="P106">
+        <v>0.1</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>92</v>
+      </c>
+      <c r="R106">
+        <v>2.7</v>
+      </c>
+      <c r="S106" t="s">
+        <v>93</v>
+      </c>
+      <c r="T106">
+        <v>91.3</v>
+      </c>
+      <c r="U106" t="s">
+        <v>93</v>
+      </c>
+      <c r="V106">
+        <v>9.5</v>
+      </c>
+      <c r="W106" t="s">
+        <v>93</v>
+      </c>
+      <c r="X106">
+        <v>133</v>
+      </c>
+      <c r="Y106" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z106">
+        <v>0.02</v>
+      </c>
+      <c r="AA106" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF106">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AG106" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL106">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AM106" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN106">
+        <v>16.5</v>
+      </c>
+      <c r="AO106" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP106">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="AQ106" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR106">
+        <v>0.02</v>
+      </c>
+      <c r="AS106" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT106">
+        <v>2.7</v>
+      </c>
+      <c r="AU106" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="107" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D107" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="H107">
+        <v>7.56</v>
+      </c>
+      <c r="I107">
+        <v>434</v>
+      </c>
+      <c r="J107">
+        <v>0.1</v>
+      </c>
+      <c r="K107" t="s">
+        <v>92</v>
+      </c>
+      <c r="L107">
+        <v>0.05</v>
+      </c>
+      <c r="M107" t="s">
+        <v>92</v>
+      </c>
+      <c r="N107">
+        <v>1</v>
+      </c>
+      <c r="O107" t="s">
+        <v>92</v>
+      </c>
+      <c r="R107">
+        <v>1.34</v>
+      </c>
+      <c r="S107" t="s">
+        <v>93</v>
+      </c>
+      <c r="T107">
+        <v>58.2</v>
+      </c>
+      <c r="U107" t="s">
+        <v>93</v>
+      </c>
+      <c r="V107">
+        <v>5.72</v>
+      </c>
+      <c r="W107" t="s">
+        <v>93</v>
+      </c>
+      <c r="X107">
+        <v>23</v>
+      </c>
+      <c r="Y107" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z107">
+        <v>0.02</v>
+      </c>
+      <c r="AA107" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD107">
+        <v>0.05</v>
+      </c>
+      <c r="AE107" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF107">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="AG107" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH107">
+        <v>0.1</v>
+      </c>
+      <c r="AI107" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL107">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AM107" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN107">
+        <v>24.3</v>
+      </c>
+      <c r="AO107" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP107">
+        <v>31</v>
+      </c>
+      <c r="AQ107" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR107">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AS107" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT107">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AU107" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="108" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="H108">
+        <v>8.18</v>
+      </c>
+      <c r="I108">
+        <v>265</v>
+      </c>
+      <c r="J108">
+        <v>0.06</v>
+      </c>
+      <c r="K108" t="s">
+        <v>92</v>
+      </c>
+      <c r="L108">
+        <v>0.01</v>
+      </c>
+      <c r="M108" t="s">
+        <v>92</v>
+      </c>
+      <c r="N108">
+        <v>7.3</v>
+      </c>
+      <c r="O108" t="s">
+        <v>93</v>
+      </c>
+      <c r="R108">
+        <v>2.9</v>
+      </c>
+      <c r="S108" t="s">
+        <v>93</v>
+      </c>
+      <c r="T108">
+        <v>29.5</v>
+      </c>
+      <c r="U108" t="s">
+        <v>93</v>
+      </c>
+      <c r="V108">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W108" t="s">
+        <v>93</v>
+      </c>
+      <c r="X108">
+        <v>39</v>
+      </c>
+      <c r="Y108" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z108">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD108">
+        <v>1E-3</v>
+      </c>
+      <c r="AE108" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF108">
+        <v>1E-3</v>
+      </c>
+      <c r="AG108" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH108">
+        <v>0.02</v>
+      </c>
+      <c r="AI108" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL108">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AM108" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN108">
+        <v>11.8</v>
+      </c>
+      <c r="AO108" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP108">
+        <v>22</v>
+      </c>
+      <c r="AQ108" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR108">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AS108" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT108">
+        <v>1</v>
+      </c>
+      <c r="AU108" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="109" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="D109" s="5">
+        <v>2022</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="H109">
+        <v>7.99</v>
+      </c>
+      <c r="J109">
+        <v>0.05</v>
+      </c>
+      <c r="K109" t="s">
+        <v>92</v>
+      </c>
+      <c r="L109">
+        <v>0.02</v>
+      </c>
+      <c r="M109" t="s">
+        <v>92</v>
+      </c>
+      <c r="N109">
+        <v>16.5</v>
+      </c>
+      <c r="O109" t="s">
+        <v>93</v>
+      </c>
+      <c r="R109">
+        <v>3.9</v>
+      </c>
+      <c r="S109" t="s">
+        <v>93</v>
+      </c>
+      <c r="T109">
+        <v>46.3</v>
+      </c>
+      <c r="U109" t="s">
+        <v>93</v>
+      </c>
+      <c r="V109">
+        <v>22.8</v>
+      </c>
+      <c r="W109" t="s">
+        <v>93</v>
+      </c>
+      <c r="X109">
+        <v>14.1</v>
+      </c>
+      <c r="Y109" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z109">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AA109" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD109">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AE109" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF109">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG109" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH109">
+        <v>0.02</v>
+      </c>
+      <c r="AI109" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL109">
+        <v>2E-3</v>
+      </c>
+      <c r="AM109" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN109">
+        <v>12.2</v>
+      </c>
+      <c r="AO109" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP109">
+        <v>14.1</v>
+      </c>
+      <c r="AQ109" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR109">
+        <v>0.02</v>
+      </c>
+      <c r="AS109" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="110" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="H110">
+        <f>AVERAGE(8,9)</f>
+        <v>8.5</v>
+      </c>
+      <c r="I110">
+        <f>AVERAGE(180,320)</f>
+        <v>250</v>
+      </c>
+      <c r="J110">
+        <v>0.04</v>
+      </c>
+      <c r="K110" t="s">
+        <v>92</v>
+      </c>
+      <c r="L110">
+        <v>0.1</v>
+      </c>
+      <c r="M110" t="s">
+        <v>92</v>
+      </c>
+      <c r="N110">
+        <f>AVERAGE(2,10)</f>
+        <v>6</v>
+      </c>
+      <c r="O110" t="s">
+        <v>93</v>
+      </c>
+      <c r="R110">
+        <f>AVERAGE(1,3)</f>
+        <v>2</v>
+      </c>
+      <c r="S110" t="s">
+        <v>93</v>
+      </c>
+      <c r="T110">
+        <f>AVERAGE(10,50)</f>
+        <v>30</v>
+      </c>
+      <c r="U110" t="s">
+        <v>93</v>
+      </c>
+      <c r="V110">
+        <f>AVERAGE(2,8)</f>
+        <v>5</v>
+      </c>
+      <c r="W110" t="s">
+        <v>93</v>
+      </c>
+      <c r="X110">
+        <f>AVERAGE(20,35)</f>
+        <v>27.5</v>
+      </c>
+      <c r="Y110" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z110">
+        <v>0.02</v>
+      </c>
+      <c r="AA110" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD110">
+        <v>0.01</v>
+      </c>
+      <c r="AE110" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF110">
+        <v>0.01</v>
+      </c>
+      <c r="AG110" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN110">
+        <f>AVERAGE(5,15)</f>
+        <v>10</v>
+      </c>
+      <c r="AO110" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP110">
+        <f>AVERAGE(10,25)</f>
+        <v>17.5</v>
+      </c>
+      <c r="AQ110" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR110">
+        <v>0.05</v>
+      </c>
+      <c r="AS110" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="111" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D111" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="H111">
+        <v>7.93</v>
+      </c>
+      <c r="I111">
+        <v>261</v>
+      </c>
+      <c r="J111">
+        <v>0.01</v>
+      </c>
+      <c r="K111" t="s">
+        <v>92</v>
+      </c>
+      <c r="L111">
+        <v>0.01</v>
+      </c>
+      <c r="M111" t="s">
+        <v>92</v>
+      </c>
+      <c r="N111">
+        <v>0.5</v>
+      </c>
+      <c r="O111" t="s">
+        <v>92</v>
+      </c>
+      <c r="R111">
+        <v>0.8</v>
+      </c>
+      <c r="S111" t="s">
+        <v>93</v>
+      </c>
+      <c r="T111">
+        <v>42.1</v>
+      </c>
+      <c r="U111" t="s">
+        <v>93</v>
+      </c>
+      <c r="V111">
+        <v>3.8</v>
+      </c>
+      <c r="W111" t="s">
+        <v>93</v>
+      </c>
+      <c r="X111">
+        <v>13.6</v>
+      </c>
+      <c r="Y111" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z111">
+        <v>0.01</v>
+      </c>
+      <c r="AA111" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF111">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG111" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN111">
+        <v>5.3</v>
+      </c>
+      <c r="AO111" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP111">
+        <v>8.6</v>
+      </c>
+      <c r="AQ111" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR111">
+        <v>0.02</v>
+      </c>
+      <c r="AS111" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT111">
+        <v>0.6</v>
+      </c>
+      <c r="AU111" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="112" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D112" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="H112">
+        <v>8.07</v>
+      </c>
+      <c r="I112">
+        <v>122</v>
+      </c>
+      <c r="J112">
+        <v>0.01</v>
+      </c>
+      <c r="K112" t="s">
+        <v>92</v>
+      </c>
+      <c r="L112">
+        <v>0.01</v>
+      </c>
+      <c r="M112" t="s">
+        <v>92</v>
+      </c>
+      <c r="N112">
+        <v>2.4</v>
+      </c>
+      <c r="O112" t="s">
+        <v>93</v>
+      </c>
+      <c r="R112">
+        <v>1.4</v>
+      </c>
+      <c r="S112" t="s">
+        <v>93</v>
+      </c>
+      <c r="T112">
+        <v>13.7</v>
+      </c>
+      <c r="U112" t="s">
+        <v>93</v>
+      </c>
+      <c r="V112">
+        <v>5.4</v>
+      </c>
+      <c r="W112" t="s">
+        <v>93</v>
+      </c>
+      <c r="X112">
+        <v>4.8</v>
+      </c>
+      <c r="Y112" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z112">
+        <v>0.01</v>
+      </c>
+      <c r="AA112" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF112">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG112" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN112">
+        <v>0.7</v>
+      </c>
+      <c r="AO112" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP112">
+        <v>1.9</v>
+      </c>
+      <c r="AQ112" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR112">
+        <v>0.02</v>
+      </c>
+      <c r="AS112" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT112">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AU112" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="113" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D113" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="H113">
+        <v>7.79</v>
+      </c>
+      <c r="I113">
+        <v>413</v>
+      </c>
+      <c r="J113">
+        <v>0.01</v>
+      </c>
+      <c r="K113" t="s">
+        <v>92</v>
+      </c>
+      <c r="L113">
+        <v>0.01</v>
+      </c>
+      <c r="M113" t="s">
+        <v>92</v>
+      </c>
+      <c r="N113">
+        <v>2.5</v>
+      </c>
+      <c r="O113" t="s">
+        <v>93</v>
+      </c>
+      <c r="R113">
+        <v>0.8</v>
+      </c>
+      <c r="S113" t="s">
+        <v>93</v>
+      </c>
+      <c r="T113">
+        <v>61.8</v>
+      </c>
+      <c r="U113" t="s">
+        <v>93</v>
+      </c>
+      <c r="V113">
+        <v>12.3</v>
+      </c>
+      <c r="W113" t="s">
+        <v>93</v>
+      </c>
+      <c r="X113">
+        <v>20.5</v>
+      </c>
+      <c r="Y113" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z113">
+        <v>0.01</v>
+      </c>
+      <c r="AA113" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD113">
+        <v>2E-3</v>
+      </c>
+      <c r="AE113" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF113">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="AG113" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH113">
+        <v>0.03</v>
+      </c>
+      <c r="AI113" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL113">
+        <v>1E-3</v>
+      </c>
+      <c r="AM113" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN113">
+        <v>4.7</v>
+      </c>
+      <c r="AO113" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP113">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AQ113" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR113">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AS113" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT113">
+        <v>0.69</v>
+      </c>
+      <c r="AU113" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="114" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D114" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="H114">
+        <v>7.7</v>
+      </c>
+      <c r="I114">
+        <v>336</v>
+      </c>
+      <c r="J114">
+        <v>0.02</v>
+      </c>
+      <c r="K114" t="s">
+        <v>92</v>
+      </c>
+      <c r="L114">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M114" t="s">
+        <v>92</v>
+      </c>
+      <c r="N114">
+        <v>6.1</v>
+      </c>
+      <c r="O114" t="s">
+        <v>93</v>
+      </c>
+      <c r="P114">
+        <v>0.01</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>92</v>
+      </c>
+      <c r="R114">
+        <v>0.44</v>
+      </c>
+      <c r="S114" t="s">
+        <v>93</v>
+      </c>
+      <c r="T114">
+        <v>53.7</v>
+      </c>
+      <c r="U114" t="s">
+        <v>93</v>
+      </c>
+      <c r="V114">
+        <v>13.4</v>
+      </c>
+      <c r="W114" t="s">
+        <v>93</v>
+      </c>
+      <c r="X114">
+        <v>6.3</v>
+      </c>
+      <c r="Y114" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z114">
+        <v>0.01</v>
+      </c>
+      <c r="AA114" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF114">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG114" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN114">
+        <v>4.47</v>
+      </c>
+      <c r="AO114" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT114">
+        <v>0.6</v>
+      </c>
+      <c r="AU114" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="115" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="D115" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="H115">
+        <v>7.4</v>
+      </c>
+      <c r="I115">
+        <v>640</v>
+      </c>
+      <c r="Z115" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="AA115" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB115" s="16">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AC115" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD115" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="AE115" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF115" s="16">
+        <v>2E-3</v>
+      </c>
+      <c r="AG115" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH115" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="AI115" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL115" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="AM115" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR115" s="16">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AS115" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="116" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="D116" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="H116">
+        <v>7.9</v>
+      </c>
+      <c r="I116">
+        <v>292</v>
+      </c>
+      <c r="J116">
+        <v>0.01</v>
+      </c>
+      <c r="K116" t="s">
+        <v>92</v>
+      </c>
+      <c r="L116">
+        <v>1E-3</v>
+      </c>
+      <c r="M116" t="s">
+        <v>92</v>
+      </c>
+      <c r="N116">
+        <v>3.7</v>
+      </c>
+      <c r="O116" t="s">
+        <v>93</v>
+      </c>
+      <c r="P116">
+        <v>0.01</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>92</v>
+      </c>
+      <c r="R116">
+        <v>0.3</v>
+      </c>
+      <c r="S116" t="s">
+        <v>93</v>
+      </c>
+      <c r="T116">
+        <v>40.4</v>
+      </c>
+      <c r="U116" t="s">
+        <v>93</v>
+      </c>
+      <c r="V116">
+        <v>13</v>
+      </c>
+      <c r="W116" t="s">
+        <v>93</v>
+      </c>
+      <c r="X116">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Y116" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z116" s="16">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AA116" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB116" s="16">
+        <v>1.0300000000000001E-3</v>
+      </c>
+      <c r="AC116" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD116" s="16">
+        <v>4.4000000000000002E-4</v>
+      </c>
+      <c r="AE116" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF116" s="16">
+        <v>3.1E-4</v>
+      </c>
+      <c r="AG116" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH116" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="AI116" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL116" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="AM116" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN116">
+        <v>0.6</v>
+      </c>
+      <c r="AO116" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP116">
+        <v>0.7</v>
+      </c>
+      <c r="AQ116" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR116" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="AS116" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="117" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D117" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="H117">
+        <v>7.1</v>
+      </c>
+      <c r="I117">
+        <v>717</v>
+      </c>
+      <c r="J117">
+        <v>0.03</v>
+      </c>
+      <c r="K117" t="s">
+        <v>92</v>
+      </c>
+      <c r="L117">
+        <v>0.01</v>
+      </c>
+      <c r="M117" t="s">
+        <v>92</v>
+      </c>
+      <c r="N117">
+        <v>23.3</v>
+      </c>
+      <c r="O117" t="s">
+        <v>93</v>
+      </c>
+      <c r="R117">
+        <v>4.3</v>
+      </c>
+      <c r="S117" t="s">
+        <v>93</v>
+      </c>
+      <c r="T117">
+        <v>100.3</v>
+      </c>
+      <c r="U117" t="s">
+        <v>93</v>
+      </c>
+      <c r="V117">
+        <v>24.9</v>
+      </c>
+      <c r="W117" t="s">
+        <v>93</v>
+      </c>
+      <c r="X117">
+        <v>29.9</v>
+      </c>
+      <c r="Y117" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z117">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AA117" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF117">
+        <v>2E-3</v>
+      </c>
+      <c r="AG117" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN117">
+        <v>28.8</v>
+      </c>
+      <c r="AO117" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP117">
+        <v>52.2</v>
+      </c>
+      <c r="AQ117" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="118" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="D118" s="5">
+        <v>2022</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="H118">
+        <v>7.5</v>
+      </c>
+      <c r="I118">
+        <v>582</v>
+      </c>
+      <c r="J118">
+        <v>0.05</v>
+      </c>
+      <c r="K118" t="s">
+        <v>92</v>
+      </c>
+      <c r="L118">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M118" t="s">
+        <v>92</v>
+      </c>
+      <c r="N118">
+        <v>3.4</v>
+      </c>
+      <c r="O118" t="s">
+        <v>93</v>
+      </c>
+      <c r="R118">
+        <v>2</v>
+      </c>
+      <c r="S118" t="s">
+        <v>92</v>
+      </c>
+      <c r="T118">
+        <v>87.4</v>
+      </c>
+      <c r="U118" t="s">
+        <v>93</v>
+      </c>
+      <c r="V118">
+        <v>20.9</v>
+      </c>
+      <c r="W118" t="s">
+        <v>93</v>
+      </c>
+      <c r="X118">
+        <v>143</v>
+      </c>
+      <c r="Y118" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z118">
+        <v>0.03</v>
+      </c>
+      <c r="AA118" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH118">
+        <v>0.01</v>
+      </c>
+      <c r="AI118" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN118">
+        <v>2</v>
+      </c>
+      <c r="AO118" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP118">
+        <v>2</v>
+      </c>
+      <c r="AQ118" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR118">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AS118" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT118">
+        <v>0.4</v>
+      </c>
+      <c r="AU118" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="119" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="D119" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="I119">
+        <v>830</v>
+      </c>
+      <c r="J119">
+        <v>0.03</v>
+      </c>
+      <c r="K119" t="s">
+        <v>92</v>
+      </c>
+      <c r="L119">
+        <v>0.01</v>
+      </c>
+      <c r="M119" t="s">
+        <v>92</v>
+      </c>
+      <c r="N119">
+        <v>36.4</v>
+      </c>
+      <c r="O119" t="s">
+        <v>93</v>
+      </c>
+      <c r="P119">
+        <v>0.1</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>92</v>
+      </c>
+      <c r="R119">
+        <v>1</v>
+      </c>
+      <c r="S119" t="s">
+        <v>93</v>
+      </c>
+      <c r="T119">
+        <v>137</v>
+      </c>
+      <c r="U119" t="s">
+        <v>93</v>
+      </c>
+      <c r="V119">
+        <v>23.7</v>
+      </c>
+      <c r="W119" t="s">
+        <v>93</v>
+      </c>
+      <c r="X119">
+        <v>68.8</v>
+      </c>
+      <c r="Y119" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z119">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AA119" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD119">
+        <v>1E-3</v>
+      </c>
+      <c r="AE119" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF119">
+        <v>1E-3</v>
+      </c>
+      <c r="AG119" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH119">
+        <v>0.01</v>
+      </c>
+      <c r="AI119" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL119">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="AM119" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN119">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AO119" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP119">
+        <v>27.3</v>
+      </c>
+      <c r="AQ119" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR119">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AS119" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT119">
+        <v>0.5</v>
+      </c>
+      <c r="AU119" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="120" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D120" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="H120">
+        <v>8.4</v>
+      </c>
+      <c r="J120">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K120" t="s">
+        <v>93</v>
+      </c>
+      <c r="L120">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="M120" t="s">
+        <v>92</v>
+      </c>
+      <c r="R120">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S120" t="s">
+        <v>93</v>
+      </c>
+      <c r="T120">
+        <v>23</v>
+      </c>
+      <c r="U120" t="s">
+        <v>93</v>
+      </c>
+      <c r="V120">
+        <v>4.7</v>
+      </c>
+      <c r="W120" t="s">
+        <v>93</v>
+      </c>
+      <c r="X120">
+        <v>46</v>
+      </c>
+      <c r="Y120" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z120">
+        <v>0.01</v>
+      </c>
+      <c r="AA120" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD120">
+        <v>1E-3</v>
+      </c>
+      <c r="AE120" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF120">
+        <v>1E-3</v>
+      </c>
+      <c r="AG120" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN120">
+        <v>12</v>
+      </c>
+      <c r="AO120" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP120">
+        <v>14</v>
+      </c>
+      <c r="AQ120" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR120">
+        <v>0.02</v>
+      </c>
+      <c r="AS120" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT120">
+        <v>3.7</v>
+      </c>
+      <c r="AU120" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="121" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="D121" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="H121">
+        <v>8.4</v>
+      </c>
+      <c r="J121">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K121" t="s">
+        <v>93</v>
+      </c>
+      <c r="L121">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="M121" t="s">
+        <v>92</v>
+      </c>
+      <c r="R121">
+        <v>2.8</v>
+      </c>
+      <c r="S121" t="s">
+        <v>93</v>
+      </c>
+      <c r="T121">
+        <v>35</v>
+      </c>
+      <c r="U121" t="s">
+        <v>93</v>
+      </c>
+      <c r="V121">
+        <v>5.4</v>
+      </c>
+      <c r="W121" t="s">
+        <v>93</v>
+      </c>
+      <c r="X121">
+        <v>48</v>
+      </c>
+      <c r="Y121" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z121">
+        <v>0.01</v>
+      </c>
+      <c r="AA121" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD121">
+        <v>1E-3</v>
+      </c>
+      <c r="AE121" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF121">
+        <v>1E-3</v>
+      </c>
+      <c r="AG121" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN121">
+        <v>15</v>
+      </c>
+      <c r="AO121" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP121">
+        <v>19</v>
+      </c>
+      <c r="AQ121" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR121">
+        <v>0.02</v>
+      </c>
+      <c r="AS121" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT121">
+        <v>4.2</v>
+      </c>
+      <c r="AU121" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="122" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D122" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="H122">
+        <v>7.8</v>
+      </c>
+      <c r="I122">
+        <v>19.5</v>
+      </c>
+      <c r="J122" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="K122" t="s">
+        <v>92</v>
+      </c>
+      <c r="L122" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="M122" t="s">
+        <v>92</v>
+      </c>
+      <c r="N122" s="16">
+        <v>0.41</v>
+      </c>
+      <c r="O122" t="s">
+        <v>93</v>
+      </c>
+      <c r="P122">
+        <f>0.005/0.33</f>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>92</v>
+      </c>
+      <c r="R122">
+        <v>1.2</v>
+      </c>
+      <c r="S122" t="s">
+        <v>93</v>
+      </c>
+      <c r="T122">
+        <v>18</v>
+      </c>
+      <c r="U122" t="s">
+        <v>93</v>
+      </c>
+      <c r="V122">
+        <v>1.5</v>
+      </c>
+      <c r="W122" t="s">
+        <v>93</v>
+      </c>
+      <c r="X122">
+        <v>26</v>
+      </c>
+      <c r="Y122" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z122" s="16">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="AA122" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD122">
+        <v>0.3</v>
+      </c>
+      <c r="AE122" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF122">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AG122" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH122" s="16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AI122" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN122">
+        <v>19</v>
+      </c>
+      <c r="AO122" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP122">
+        <v>9</v>
+      </c>
+      <c r="AQ122" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR122">
+        <v>0.02</v>
+      </c>
+      <c r="AS122" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT122">
+        <v>2</v>
+      </c>
+      <c r="AU122" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="J1:X1"/>

</xml_diff>